<commit_message>
feature 3.menu 80% done
</commit_message>
<xml_diff>
--- a/data/productInfo.xlsx
+++ b/data/productInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>productName</t>
   </si>
@@ -25,13 +25,25 @@
     <t>productAmount</t>
   </si>
   <si>
-    <t>Coke</t>
-  </si>
-  <si>
-    <t>Angkor</t>
-  </si>
-  <si>
-    <t>donut</t>
+    <t>productCategory</t>
+  </si>
+  <si>
+    <t>Coca</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>Donut</t>
+  </si>
+  <si>
+    <t>red red</t>
   </si>
 </sst>
 </file>
@@ -341,13 +353,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -357,38 +369,64 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>45</v>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1.5</v>
       </c>
       <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="C5">
         <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>